<commit_message>
Updated Master data as per 16th May Refresh
</commit_message>
<xml_diff>
--- a/docs/requirements/Master Data Tables - Test Data/master-reg_center_user.xlsx
+++ b/docs/requirements/Master Data Tables - Test Data/master-reg_center_user.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1045476\Desktop\DB Updated Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0A970B69-7D8E-4AAD-A830-F607E5C6E8F2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8EF17727-FB34-4FA0-9F9D-3E32D39E4BFD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="9">
   <si>
     <t>regcntr_id</t>
   </si>
@@ -887,10 +887,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1555,6 +1555,66 @@
         <v>8</v>
       </c>
     </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>10005</v>
+      </c>
+      <c r="B34">
+        <v>110033</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" t="b">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>10005</v>
+      </c>
+      <c r="B35">
+        <v>110034</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" t="b">
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>10005</v>
+      </c>
+      <c r="B36">
+        <v>110035</v>
+      </c>
+      <c r="C36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" t="b">
+        <v>1</v>
+      </c>
+      <c r="E36" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>